<commit_message>
playing with o blindness heuristics
</commit_message>
<xml_diff>
--- a/stats/heuristics_fitted_combinations_20052018.xlsx
+++ b/stats/heuristics_fitted_combinations_20052018.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="27795" windowHeight="11310" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="27795" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics_fitted_combinations_" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="fewer" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="24" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -4855,7 +4855,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -17700,7 +17700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -17832,7 +17832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G347"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>

</xml_diff>